<commit_message>
database changes based on Sebastien's review - replaced vote table with post_vote and comment_vote; fixed some typos; added db_Create_User.sql
</commit_message>
<xml_diff>
--- a/src/main/database/db_SchemaSpecification.xlsx
+++ b/src/main/database/db_SchemaSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="181">
   <si>
     <t>Column name</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>UI converts datetime values to local time zone.</t>
-  </si>
-  <si>
-    <t>vote: record user's vote for posts and comments (relationship between user &amp; post, user &amp; comment)</t>
   </si>
   <si>
     <t>user_follows: posts, sdg, or tags followed by each user (relationship between user and user, post, or tag)</t>
@@ -582,6 +579,12 @@
   </si>
   <si>
     <t>The schema is subject to change after we know how to use MapBox API.</t>
+  </si>
+  <si>
+    <t>post_vote: record user's vote for posts (relationship between user &amp; post)</t>
+  </si>
+  <si>
+    <t>comment_vote: record user's vote for comments (relationship between user &amp; comment)</t>
   </si>
 </sst>
 </file>
@@ -715,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -750,11 +753,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1060,10 +1064,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,20 +1088,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
         <v>151</v>
-      </c>
-      <c r="B3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1112,7 +1116,7 @@
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1122,12 +1126,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1147,7 +1151,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -1162,12 +1166,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -1175,39 +1179,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>29</v>
+    <row r="24" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>31</v>
+      <c r="A29" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -1215,14 +1219,19 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1265,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1273,13 +1282,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1288,10 +1297,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -1303,64 +1312,64 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>120</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1405,7 +1414,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1413,13 +1422,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1428,10 +1437,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -1443,44 +1452,44 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1522,7 +1531,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1530,13 +1539,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1545,10 +1554,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -1560,44 +1569,44 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1648,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1647,13 +1656,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1662,10 +1671,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>12</v>
@@ -1677,103 +1686,103 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="A13" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,13 +1835,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1841,10 +1850,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -1856,64 +1865,64 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1947,18 +1956,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2005,7 +2014,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -2016,13 +2025,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2031,10 +2040,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2046,25 +2055,25 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -2074,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -2082,10 +2091,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10">
@@ -2095,10 +2104,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10">
@@ -2108,10 +2117,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2119,23 +2128,23 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2146,10 +2155,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -2159,10 +2168,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -2172,23 +2181,23 @@
         <v>9</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2198,7 +2207,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2206,40 +2215,40 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2281,7 +2290,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2289,13 +2298,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2304,10 +2313,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2319,35 +2328,35 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10"/>
@@ -2355,10 +2364,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="10"/>
@@ -2366,23 +2375,23 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2390,10 +2399,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2401,23 +2410,23 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -2425,50 +2434,50 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2514,7 +2523,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2522,13 +2531,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2537,10 +2546,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2552,66 +2561,66 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>86</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2653,7 +2662,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2661,13 +2670,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2676,10 +2685,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2691,29 +2700,29 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="17"/>
     </row>
@@ -2756,7 +2765,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2764,13 +2773,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2779,10 +2788,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2794,64 +2803,64 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -2895,7 +2904,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2903,13 +2912,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2918,10 +2927,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -2933,66 +2942,66 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3036,7 +3045,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3044,13 +3053,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -3059,10 +3068,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -3074,51 +3083,51 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>114</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>115</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3162,7 +3171,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3170,13 +3179,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -3185,10 +3194,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
@@ -3200,51 +3209,51 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>

</xml_diff>